<commit_message>
Updated with code used to get results for the 6_7-8_23 update doc
</commit_message>
<xml_diff>
--- a/Data/EconomicData/MonthlyEggs-BLS.xlsx
+++ b/Data/EconomicData/MonthlyEggs-BLS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\CodingProjectsStuff\2023SummerResearch-Inflation\COVID-Inflation\Data\EconomicData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BA32B6-CAF0-4B84-B167-7D5E6A92026B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCE821A-0094-4121-8EAF-95859A147CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -188,9 +188,9 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BLS Data Series'!$C$1</c:f>
+              <c:f>'BLS Data Series'!$C$1:$C$2</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>EggPrice%Change</c:v>
                 </c:pt>
@@ -209,847 +209,1693 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'BLS Data Series'!$A$3:$A$281</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="279"/>
+                <c:pt idx="0">
+                  <c:v>36557</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36586</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36617</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36647</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36678</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36708</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36739</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36770</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36831</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36861</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36892</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36923</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>36951</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36982</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>37012</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>37043</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>37073</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>37104</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>37135</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>37165</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>37196</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>37226</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>37257</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>37288</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>37316</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>37347</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>37377</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>37408</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>37438</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>37469</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>37500</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>37530</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>37561</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>37591</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>37622</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37653</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37681</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>37712</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>37742</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>37773</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>37803</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>37834</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>37865</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>37895</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>37926</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>37956</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>37987</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>38018</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>38047</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>38078</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>38108</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>38139</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>38169</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>38200</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>38231</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>38261</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>38292</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>38322</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>38353</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>38384</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>38412</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>38443</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>38473</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>38504</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>38534</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>38565</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>38596</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>38626</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>38657</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>38687</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>38718</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>38749</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>38777</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>38808</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>38838</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>38869</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>38899</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>38930</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>38961</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>38991</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>39022</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>39052</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>39083</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>39114</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>39142</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>39173</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>39203</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>39234</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>39264</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>39295</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>39326</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>39356</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>39387</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>39417</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>39448</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>39479</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>39508</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>39539</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>39569</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>39600</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>39630</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>39661</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>39692</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>39722</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>39753</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>39783</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>39814</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>39845</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>39873</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>39904</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>39934</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>39965</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>39995</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>40026</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>40057</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>40087</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>40118</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>40148</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>40179</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>40210</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>40238</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>40269</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>40299</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>40330</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>40360</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>40391</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>40422</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>40452</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>40483</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>40513</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>40544</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>40575</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>40603</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>40634</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>40664</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>40695</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>40725</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>40756</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>40787</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>40817</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>40848</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>40878</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>40909</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>40940</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>41000</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>41030</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>41061</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>41091</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>41122</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>41153</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>41183</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>41214</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>41244</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>41275</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>41306</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>41334</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>41365</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>41395</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>41426</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>41456</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>41487</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>41518</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>41548</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>41579</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>41609</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>41640</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>41671</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>41699</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>41730</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>41760</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>41791</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>41821</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>41852</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>41883</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>41913</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>41944</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>41974</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>42005</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>42036</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>42064</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>42095</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>42125</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>42156</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>42186</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>42217</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>42248</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>42278</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>42309</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>42339</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>42370</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>42401</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>42430</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>42461</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>42491</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>42522</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>42552</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>42583</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>42614</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>42644</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>42675</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>42705</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>42736</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>42767</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>42795</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>42826</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>42856</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>42887</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>42917</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>42948</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>42979</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>43009</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>43040</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>43070</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>43132</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>43160</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>43252</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>43282</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>43313</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>43344</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>43374</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>43405</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>43435</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>43466</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>43497</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>43525</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>43556</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>43617</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>43647</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>43678</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>43709</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>43739</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>43770</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>43800</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>43831</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>43891</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>44378</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>44409</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>44440</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>44470</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>44835</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>44866</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>44896</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>44927</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>44958</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>44986</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>45017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BLS Data Series'!$C$2:$C$281</c:f>
+              <c:f>'BLS Data Series'!$C$3:$C$281</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="280"/>
+                <c:ptCount val="279"/>
+                <c:pt idx="0">
+                  <c:v>-1.3333333333333346</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.3333333333333346</c:v>
+                  <c:v>-3.2224532224532134</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.2224532224532134</c:v>
+                  <c:v>0.85929108485498351</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.85929108485498351</c:v>
+                  <c:v>-9.2651757188498376</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-9.2651757188498376</c:v>
+                  <c:v>-1.6431924882629123</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.6431924882629123</c:v>
+                  <c:v>3.5799522673031063</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5799522673031063</c:v>
+                  <c:v>2.8801843317972375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8801843317972375</c:v>
+                  <c:v>3.0235162374020184</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0235162374020184</c:v>
+                  <c:v>0.32608695652173941</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.32608695652173941</c:v>
+                  <c:v>-2.2751895991332631</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2.2751895991332631</c:v>
+                  <c:v>6.3192904656319211</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.3192904656319211</c:v>
+                  <c:v>5.4223149113659996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.4223149113659996</c:v>
+                  <c:v>-6.7260138476755644</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-6.7260138476755644</c:v>
+                  <c:v>-6.0445387062566223</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-6.0445387062566223</c:v>
+                  <c:v>16.02708803611738</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.02708803611738</c:v>
+                  <c:v>-14.299610894941637</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-14.299610894941637</c:v>
+                  <c:v>4.4267877412031824</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.4267877412031824</c:v>
+                  <c:v>-6.3043478260869614</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-6.3043478260869614</c:v>
+                  <c:v>7.7726218097447868</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.7726218097447868</c:v>
+                  <c:v>-1.3993541442411206</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-1.3993541442411206</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>2.0742358078602638</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-1.0695187165775408</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.1891891891891815</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.3638232271325816</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.70281124497990921</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.3868394815553389</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-4.7755491881566314</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-2.2066198595787383</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.5384615384615399</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.3636363636363589</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.18993352326685678</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-1.5165876777251199</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.9461020211742208</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.8888888888888751</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-8.5034013605432821E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.1914893617021287</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.6820857863751066</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-6.4516129032258114</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-10.786914235190107</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>18.830525272547092</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-4.0867389491242827</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>11.043478260869566</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1.5661707126076756</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.8074781225139365</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8.8721804511278108</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7.665745856353591</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.89801154586273346</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.63572790845518168</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.6531901452937485</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-3.8769230769230738</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-12.163892445582583</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-4.4460641399417034</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-4.4241037376048853</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.9154030327214702</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-10.336726703210642</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-4.8908296943231484</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-0.36730945821854949</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>10.506912442396322</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.000834028356965</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6.0280759702724982</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-11.838006230529604</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.8268551236749144</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.8041237113402175</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-3.8818565400843914</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.2827041264266921</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>8.583690987123517E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>9.6912521440823323</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-1.1727912431587102</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.186708860759486</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5.5512118842846112</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.3333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-8.3505866114561762</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-1.9578313253012065</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-1.4592933947772755</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-6.001558846453622</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2.9850746268656745</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-2.3349436392914584</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.5556471558120295</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.80385852090032217</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.23923444976075692</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>7.716785998408926</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>13.958641063515497</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.38885288399222329</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>12.717882504841837</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-6.4146620847651841</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-1.1015911872704893</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-6.9306930693069368</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-8.710106382978724</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>9.3954843408594328</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>8.7882822902796196</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>11.689106487148107</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-2.9589041095890436</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>5.1383399209486278</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>12.728249194414612</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.6207717960933596</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-0.32183908045975512</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.6143911439114251</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-6.0826146164321342</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-6.7182213629772853</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-0.51813471502590724</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>4.7395833333333437</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-7.8070611636002001</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>6.6882416396979432</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-6.0667340748230476</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-1.076426264800862</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-0.21762785636561499</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.87241003271537698</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-2.9729729729729817</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-5.6824512534818874</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>4.7844063792085025</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-15.388951521984223</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1.8654230512991359</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>-2.2236756049705564</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>9.1638795986621933</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>-0.30637254901960131</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>-1.966810079901661</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>6.8965517241379377</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>3.9296187683284427</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.95936794582392237</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>4.6394633873672548</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>-2.6709401709401734</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>-2.3600439077936417</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>-14.390106801573918</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>-1.9041365725541639</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>-3.547523427041495</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>5.412907702984028</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>15.404871626069783</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>-16.942384483742153</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>15.041208791208796</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>7.0447761194029779</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.72504182933631467</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>-5.426356589147292</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>1.4051522248243571</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>-0.28868360277135641</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>-2.026635784597576</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>-0.53191489361701516</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>-2.1390374331550821</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>3.885853066180939</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>13.793103448275861</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>-3.9034411915767881</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>-1.870657402458574</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>2.0697167755991304</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>3.4685165421558133</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>-7.2717895822588972</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>-1.3348164627363748</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>3.1003382187147652</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>-7.5451066156369553</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>-1.241868716735667</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>-1.3173652694610789</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>14.320388349514563</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.26539278131635435</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>3.7586024351508707</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.15306122448980172</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>2.2414671421293955</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>-3.6870951669157979</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>1.655457837558201</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>-2.035623409669213</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>-0.3636363636363697</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>-2.5026068821689167</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>-0.58823529411765352</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>-1.3986013986013999</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.27277686852155569</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>3.2100108813928148</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>1.4760147601476028</c:v>
+                </c:pt>
+                <c:pt idx="165">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.0742358078602638</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-1.0695187165775408</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5.1891891891891815</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.3638232271325816</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.70281124497990921</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4.3868394815553389</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-4.7755491881566314</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>-2.2066198595787383</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.5384615384615399</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>6.3636363636363589</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.18993352326685678</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>-1.5165876777251199</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>3.9461020211742208</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>8.8888888888888751</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>-8.5034013605432821E-2</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1.1914893617021287</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1.6820857863751066</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>-6.4516129032258114</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>-10.786914235190107</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>18.830525272547092</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>-4.0867389491242827</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>11.043478260869566</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>-1.5661707126076756</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>5.8074781225139365</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>8.8721804511278108</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>7.665745856353591</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.89801154586273346</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.63572790845518168</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>2.6531901452937485</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>-3.8769230769230738</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>-12.163892445582583</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>-4.4460641399417034</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>-4.4241037376048853</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>1.9154030327214702</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>-10.336726703210642</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>-4.8908296943231484</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>-0.36730945821854949</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>10.506912442396322</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>1.000834028356965</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>6.0280759702724982</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>-11.838006230529604</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>2.8268551236749144</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>1.8041237113402175</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>-3.8818565400843914</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>2.2827041264266921</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>8.583690987123517E-2</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>9.6912521440823323</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>-1.1727912431587102</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>1.186708860759486</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>5.5512118842846112</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>7.3333333333333304</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>-8.3505866114561762</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>-1.9578313253012065</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>-1.4592933947772755</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>-6.001558846453622</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>2.9850746268656745</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>-2.3349436392914584</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>2.5556471558120295</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.80385852090032217</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.23923444976075692</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>7.716785998408926</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>13.958641063515497</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.38885288399222329</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>12.717882504841837</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>-6.4146620847651841</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>-1.1015911872704893</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>-6.9306930693069368</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>-8.710106382978724</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>9.3954843408594328</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>8.7882822902796196</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>11.689106487148107</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>-2.9589041095890436</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>5.1383399209486278</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>12.728249194414612</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>3.6207717960933596</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>-0.32183908045975512</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>1.6143911439114251</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>-6.0826146164321342</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>-6.7182213629772853</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>-0.51813471502590724</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>4.7395833333333437</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>-7.8070611636002001</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>6.6882416396979432</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>-6.0667340748230476</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>-1.076426264800862</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>-0.21762785636561499</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.87241003271537698</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>-2.9729729729729817</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>-5.6824512534818874</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>4.7844063792085025</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>-15.388951521984223</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>1.8654230512991359</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>-2.2236756049705564</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>9.1638795986621933</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>-0.30637254901960131</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>-1.966810079901661</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>6.8965517241379377</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>3.9296187683284427</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.95936794582392237</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>4.6394633873672548</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>-2.6709401709401734</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>-2.3600439077936417</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>-14.390106801573918</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>-1.9041365725541639</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>-3.547523427041495</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>5.412907702984028</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>15.404871626069783</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>-16.942384483742153</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>15.041208791208796</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>7.0447761194029779</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>0.72504182933631467</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>-5.426356589147292</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>1.4051522248243571</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>-0.28868360277135641</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>-2.026635784597576</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>-0.53191489361701516</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>-2.1390374331550821</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>3.885853066180939</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>13.793103448275861</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>-3.9034411915767881</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>-1.870657402458574</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>2.0697167755991304</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>3.4685165421558133</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>-7.2717895822588972</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>-1.3348164627363748</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>3.1003382187147652</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>-7.5451066156369553</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>-1.241868716735667</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>-1.3173652694610789</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>14.320388349514563</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>0.26539278131635435</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>3.7586024351508707</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>0.15306122448980172</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>2.2414671421293955</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>-3.6870951669157979</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>1.655457837558201</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>-2.035623409669213</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>-0.3636363636363697</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>-2.5026068821689167</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>-0.58823529411765352</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>-1.3986013986013999</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>0.27277686852155569</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>3.2100108813928148</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>1.4760147601476028</c:v>
-                </c:pt>
                 <c:pt idx="166">
+                  <c:v>5.2467532467532338</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>-0.88845014807501455</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>-0.49800796812749049</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>3.1531531531531503</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>2.8141678796700766</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>-5.8046248230297408</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>-2.4048096192384789</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.10266940451745389</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>1.4871794871794943</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>-0.45477513895907623</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>-0.96446700507613736</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>4.1517170681701669</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>8.7598425196850371</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>-4.3891402714932113</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>-1.1831519167061009</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>2.1551724137931001</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>-3.1879981247069882</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>-4.9878934624697324</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>30.988786952089697</c:v>
+                </c:pt>
+                <c:pt idx="185">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="167">
-                  <c:v>5.2467532467532338</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>-0.88845014807501455</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>-0.49800796812749049</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>3.1531531531531503</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>2.8141678796700766</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>-5.8046248230297408</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>-2.4048096192384789</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>0.10266940451745389</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>1.4871794871794943</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>-0.45477513895907623</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>-0.96446700507613736</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>4.1517170681701669</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>8.7598425196850371</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>-4.3891402714932113</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>-1.1831519167061009</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>2.1551724137931001</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>-3.1879981247069882</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>-4.9878934624697324</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>30.988786952089697</c:v>
-                </c:pt>
                 <c:pt idx="186">
+                  <c:v>14.51361867704281</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.78151546041454745</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>-5.327039784221185</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>-5.1282051282051171</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>3.2657657657657562</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>-15.376226826608509</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>-2.6202749140893449</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>-8.2046757829730907</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>-13.839500240269103</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>-6.0791968767428886</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>-11.46080760095011</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>3.6887994634473462</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>-5.8861578266494154</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>1.0996563573883171</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>-5.5064581917063347</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>-4.9640287769784139</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>4.6934140802422455</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>15.618221258134488</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>-8.4427767354596632</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>-4.098360655737709</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.35612535612536439</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.35486160397444239</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>-5.7991513437057893</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>7.5075075075066805E-2</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>2.5506376594148561</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>4.0234089246525189</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>8.2981715893108383</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>-2.2077922077922096</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>20.517928286852584</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>-2.534435261707991</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>-0.79140757490107494</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>4.3304843304843343</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>13.653741125068269</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>-4.5170591061989365</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>-18.067438349270265</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>5.9582309582309705</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>-5.9710144927536213</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>1.7879161528976519</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.54512416717140511</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>-3.8554216867469777</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>-6.265664160401703E-2</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>-2.5705329153604968</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.19305019305018606</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>-0.83493898522799626</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>-5.246113989637303</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>-6.9036226930963753</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>-11.674008810572689</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>3.3250207813798864</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>-1.9308125502815785</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>13.453650533223946</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>-7.3029645697758481</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>9.5943837753510142</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>9.2526690391458999</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>-4.820846905537449</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>-0.82135523613963113</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>5.2449965493443651</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>32.393442622950836</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>-18.77166914314018</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>-5.2439024390243816</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>-9.8455598455598459</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>-5.210563882940753</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>1.8825301204819209</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>4.0650406504065</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>2.9829545454545485</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>2.1379310344827682</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>-1.0128291694800893</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>8.9358799454297415</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>1.7532874139010661</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>-0.30769230769230116</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>0.30864197530863535</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>1.0461538461538402</c:v>
+                </c:pt>
+                <c:pt idx="257">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="187">
-                  <c:v>14.51361867704281</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>0.78151546041454745</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>-5.327039784221185</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>-5.1282051282051171</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>3.2657657657657562</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>-15.376226826608509</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>-2.6202749140893449</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>-8.2046757829730907</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>-13.839500240269103</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>-6.0791968767428886</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>-11.46080760095011</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>3.6887994634473462</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>-5.8861578266494154</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>1.0996563573883171</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>-5.5064581917063347</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>-4.9640287769784139</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>4.6934140802422455</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>15.618221258134488</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>-8.4427767354596632</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>-4.098360655737709</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>0.35612535612536439</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>0.35486160397444239</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>-5.7991513437057893</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>7.5075075075066805E-2</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>2.5506376594148561</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>4.0234089246525189</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>8.2981715893108383</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>-2.2077922077922096</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>20.517928286852584</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>-2.534435261707991</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>-0.79140757490107494</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>4.3304843304843343</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>13.653741125068269</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>-4.5170591061989365</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>-18.067438349270265</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>5.9582309582309705</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>-5.9710144927536213</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>1.7879161528976519</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>0.54512416717140511</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>-3.8554216867469777</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>-6.265664160401703E-2</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>-2.5705329153604968</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>0.19305019305018606</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>-0.83493898522799626</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>-5.246113989637303</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>-6.9036226930963753</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>-11.674008810572689</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>3.3250207813798864</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>-1.9308125502815785</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>13.453650533223946</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>-7.3029645697758481</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>9.5943837753510142</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>9.2526690391458999</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>-4.820846905537449</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>-0.82135523613963113</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>5.2449965493443651</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>32.393442622950836</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>-18.77166914314018</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>-5.2439024390243816</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>-9.8455598455598459</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>-5.210563882940753</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>1.8825301204819209</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>4.0650406504065</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>2.9829545454545485</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>2.1379310344827682</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>-1.0128291694800893</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>8.9358799454297415</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>1.7532874139010661</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>-0.30769230769230116</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>0.30864197530863535</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>1.0461538461538402</c:v>
-                </c:pt>
                 <c:pt idx="258">
-                  <c:v>0</c:v>
+                  <c:v>4.0803897685749195</c:v>
                 </c:pt>
                 <c:pt idx="259">
-                  <c:v>4.0803897685749195</c:v>
+                  <c:v>7.3727325921591511</c:v>
                 </c:pt>
                 <c:pt idx="260">
-                  <c:v>7.3727325921591511</c:v>
+                  <c:v>-0.76294277929155385</c:v>
                 </c:pt>
                 <c:pt idx="261">
-                  <c:v>-0.76294277929155385</c:v>
+                  <c:v>-5.6562328390993946</c:v>
                 </c:pt>
                 <c:pt idx="262">
-                  <c:v>-5.6562328390993946</c:v>
+                  <c:v>4.0745052386495964</c:v>
                 </c:pt>
                 <c:pt idx="263">
-                  <c:v>4.0745052386495964</c:v>
+                  <c:v>7.8859060402684573</c:v>
                 </c:pt>
                 <c:pt idx="264">
-                  <c:v>7.8859060402684573</c:v>
+                  <c:v>3.939865215137369</c:v>
                 </c:pt>
                 <c:pt idx="265">
-                  <c:v>3.939865215137369</c:v>
+                  <c:v>2.044887780548625</c:v>
                 </c:pt>
                 <c:pt idx="266">
-                  <c:v>2.044887780548625</c:v>
+                  <c:v>23.167155425219953</c:v>
                 </c:pt>
                 <c:pt idx="267">
-                  <c:v>23.167155425219953</c:v>
+                  <c:v>13.611111111111111</c:v>
                 </c:pt>
                 <c:pt idx="268">
-                  <c:v>13.611111111111111</c:v>
+                  <c:v>-5.448829898707654</c:v>
                 </c:pt>
                 <c:pt idx="269">
-                  <c:v>-5.448829898707654</c:v>
+                  <c:v>8.4595493165866316</c:v>
                 </c:pt>
                 <c:pt idx="270">
-                  <c:v>8.4595493165866316</c:v>
+                  <c:v>6.1307901907357003</c:v>
                 </c:pt>
                 <c:pt idx="271">
-                  <c:v>6.1307901907357003</c:v>
+                  <c:v>-6.8677792041078298</c:v>
                 </c:pt>
                 <c:pt idx="272">
-                  <c:v>-6.8677792041078298</c:v>
+                  <c:v>17.815299793246034</c:v>
                 </c:pt>
                 <c:pt idx="273">
-                  <c:v>17.815299793246034</c:v>
+                  <c:v>4.9722140976893803</c:v>
                 </c:pt>
                 <c:pt idx="274">
-                  <c:v>4.9722140976893803</c:v>
+                  <c:v>18.417386458623572</c:v>
                 </c:pt>
                 <c:pt idx="275">
-                  <c:v>18.417386458623572</c:v>
+                  <c:v>13.48235294117648</c:v>
                 </c:pt>
                 <c:pt idx="276">
-                  <c:v>13.48235294117648</c:v>
+                  <c:v>-12.689197594857973</c:v>
                 </c:pt>
                 <c:pt idx="277">
-                  <c:v>-12.689197594857973</c:v>
+                  <c:v>-18.166706245547378</c:v>
                 </c:pt>
                 <c:pt idx="278">
-                  <c:v>-18.166706245547378</c:v>
-                </c:pt>
-                <c:pt idx="279">
                   <c:v>-5.1073708647707532</c:v>
                 </c:pt>
               </c:numCache>
@@ -1058,7 +1904,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3721-4507-95C9-E902EB670D1E}"/>
+              <c16:uniqueId val="{00000000-8C34-4FC6-AB87-25A77BB04953}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1071,18 +1917,18 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="470910063"/>
-        <c:axId val="470913423"/>
+        <c:axId val="1839131151"/>
+        <c:axId val="1839143631"/>
       </c:lineChart>
-      <c:catAx>
-        <c:axId val="470910063"/>
+      <c:dateAx>
+        <c:axId val="1839131151"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1118,15 +1964,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470913423"/>
+        <c:crossAx val="1839143631"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
       <c:valAx>
-        <c:axId val="470913423"/>
+        <c:axId val="1839143631"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1177,7 +2022,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="470910063"/>
+        <c:crossAx val="1839131151"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1786,23 +2631,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>7626</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>7626</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{047B7D13-69B5-C7C9-706F-82B881330FB7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11A25FD3-9CDA-B11D-3A43-4528CBD3C3C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2123,8 +2968,8 @@
   <dimension ref="A1:C281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCellId="1" sqref="C1:C1048576 A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>